<commit_message>
Changes over Presupuesto file
</commit_message>
<xml_diff>
--- a/Documentos/Presupuesto.xlsx
+++ b/Documentos/Presupuesto.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Documents\GitHub\ProyectoGranEscala\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53A6AA5-75F5-4FF9-AC1D-F6FE9356790C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C26086-5518-456B-8CDE-77E50A3CFED0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{196534AB-D60A-44F2-8B54-660C8355F8E6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="62">
   <si>
     <t>Unidad de medida</t>
   </si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t>Precio por hora de tester (Tercerizado)</t>
+  </si>
+  <si>
+    <t>Smart Green</t>
   </si>
 </sst>
 </file>
@@ -220,7 +223,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="_([$COP]\ * #,##0_);_([$COP]\ * \(#,##0\);_([$COP]\ * &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,6 +247,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -281,7 +291,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -343,13 +353,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -411,37 +430,46 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -464,6 +492,61 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>8669</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A32ED28C-D7D9-42F2-A74C-3201EEBA1E98}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1095375" cy="1094519"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -897,10 +980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41D059DC-9B60-4C67-B374-7099A088B7FA}">
-  <dimension ref="B3:M48"/>
+  <dimension ref="B1:M52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -921,757 +1004,846 @@
     <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B1" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+    </row>
+    <row r="7" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="2" t="str">
-        <f>_xlfn.CONCAT("IVA ",TEXT(I25,"0.0%"))</f>
+      <c r="K7" s="2" t="str">
+        <f>_xlfn.CONCAT("IVA ",TEXT(I29,"0.0%"))</f>
         <v>IVA 19.0%</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="22" t="s">
+    <row r="8" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="3">
-        <f>E28</f>
+      <c r="F8" s="3">
+        <f>E32</f>
         <v>90</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G8" s="4">
         <v>30000</v>
       </c>
-      <c r="H4" s="4">
-        <f>G4*F4</f>
+      <c r="H8" s="4">
+        <f>G8*F8</f>
         <v>2700000</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I8" s="3">
         <v>4</v>
       </c>
-      <c r="J4" s="12">
-        <f>H4*I4</f>
+      <c r="J8" s="12">
+        <f>H8*I8</f>
         <v>10800000</v>
       </c>
-      <c r="K4" s="12">
-        <f t="shared" ref="K4:K14" si="0">J4*$I$25</f>
+      <c r="K8" s="12">
+        <f t="shared" ref="K8:K18" si="0">J8*$I$29</f>
         <v>2052000</v>
       </c>
-      <c r="L4" s="12">
-        <f>(J4+K4)*1.3</f>
+      <c r="L8" s="12">
+        <f>(J8+K8)*1.3</f>
         <v>16707600</v>
       </c>
-      <c r="M4" s="21">
-        <f>SUM(L4:L8)</f>
+      <c r="M8" s="28">
+        <f>SUM(L8:L12)</f>
         <v>28231560</v>
       </c>
     </row>
-    <row r="5" spans="2:13" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="22"/>
-      <c r="C5" s="11" t="s">
+    <row r="9" spans="2:13" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="31"/>
+      <c r="C9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="5">
-        <f>E33</f>
+      <c r="F9" s="5">
+        <f>E37</f>
         <v>28</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G9" s="6">
         <v>45000</v>
       </c>
-      <c r="H5" s="14">
-        <f t="shared" ref="H5:H14" si="1">G5*F5</f>
+      <c r="H9" s="14">
+        <f t="shared" ref="H9:H18" si="1">G9*F9</f>
         <v>1260000</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I9" s="5">
         <v>1</v>
       </c>
-      <c r="J5" s="6">
-        <f t="shared" ref="J5:J11" si="2">H5*I5</f>
+      <c r="J9" s="6">
+        <f t="shared" ref="J9:J15" si="2">H9*I9</f>
         <v>1260000</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K9" s="6">
         <f t="shared" si="0"/>
         <v>239400</v>
       </c>
-      <c r="L5" s="6">
-        <f>J5+K5</f>
+      <c r="L9" s="6">
+        <f>J9+K9</f>
         <v>1499400</v>
       </c>
-      <c r="M5" s="21"/>
-    </row>
-    <row r="6" spans="2:13" s="20" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="22"/>
-      <c r="C6" s="17" t="s">
+      <c r="M9" s="28"/>
+    </row>
+    <row r="10" spans="2:13" s="20" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="31"/>
+      <c r="C10" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D10" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E10" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="18">
-        <f>E43</f>
+      <c r="F10" s="18">
+        <f>E47</f>
         <v>90</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G10" s="13">
         <v>27000</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H10" s="19">
         <f t="shared" si="1"/>
         <v>2430000</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I10" s="18">
         <v>1</v>
       </c>
-      <c r="J6" s="13">
-        <f t="shared" ref="J6" si="3">H6*I6</f>
+      <c r="J10" s="13">
+        <f t="shared" ref="J10" si="3">H10*I10</f>
         <v>2430000</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K10" s="13">
         <f t="shared" si="0"/>
         <v>461700</v>
       </c>
-      <c r="L6" s="13">
-        <f>(J6+K6)*1.3</f>
+      <c r="L10" s="13">
+        <f>(J10+K10)*1.3</f>
         <v>3759210</v>
       </c>
-      <c r="M6" s="21"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="22"/>
-      <c r="C7" s="11" t="s">
+      <c r="M10" s="28"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="31"/>
+      <c r="C11" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="5">
-        <f>E48</f>
+      <c r="F11" s="5">
+        <f>E52</f>
         <v>39</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G11" s="6">
         <v>25000</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H11" s="14">
         <f t="shared" si="1"/>
         <v>975000</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I11" s="5">
         <v>3</v>
       </c>
-      <c r="J7" s="6">
-        <f t="shared" ref="J7" si="4">H7*I7</f>
+      <c r="J11" s="6">
+        <f t="shared" ref="J11" si="4">H11*I11</f>
         <v>2925000</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K11" s="6">
         <f t="shared" si="0"/>
         <v>555750</v>
       </c>
-      <c r="L7" s="6">
-        <f t="shared" ref="L7:L14" si="5">J7+K7</f>
+      <c r="L11" s="6">
+        <f t="shared" ref="L11:L18" si="5">J11+K11</f>
         <v>3480750</v>
       </c>
-      <c r="M7" s="21"/>
-    </row>
-    <row r="8" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="22"/>
-      <c r="C8" s="3" t="s">
+      <c r="M11" s="28"/>
+    </row>
+    <row r="12" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="31"/>
+      <c r="C12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="3">
-        <f>E38</f>
+      <c r="F12" s="3">
+        <f>E42</f>
         <v>45</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G12" s="12">
         <v>40000</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H12" s="4">
         <f t="shared" si="1"/>
         <v>1800000</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I12" s="3">
         <v>1</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J12" s="12">
         <f t="shared" si="2"/>
         <v>1800000</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K12" s="13">
         <f t="shared" si="0"/>
         <v>342000</v>
       </c>
-      <c r="L8" s="13">
-        <f>(J8+K8)*1.3</f>
+      <c r="L12" s="13">
+        <f>(J12+K12)*1.3</f>
         <v>2784600</v>
       </c>
-      <c r="M8" s="21"/>
-    </row>
-    <row r="9" spans="2:13" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="22" t="s">
+      <c r="M12" s="28"/>
+    </row>
+    <row r="13" spans="2:13" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F13" s="5">
         <v>1</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G13" s="6">
         <v>200000</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H13" s="14">
         <f t="shared" si="1"/>
         <v>200000</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I13" s="5">
         <v>1</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J13" s="6">
         <f t="shared" si="2"/>
         <v>200000</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K13" s="6">
         <f t="shared" si="0"/>
         <v>38000</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L13" s="6">
         <f t="shared" si="5"/>
         <v>238000</v>
       </c>
-      <c r="M9" s="21">
-        <f>SUM(L9:L11)</f>
+      <c r="M13" s="28">
+        <f>SUM(L13:L15)</f>
         <v>2542930.04</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="22"/>
-      <c r="C10" s="3" t="s">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="31"/>
+      <c r="C14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F14" s="3">
         <v>1</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G14" s="12">
         <v>189076</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H14" s="4">
         <f t="shared" si="1"/>
         <v>189076</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I14" s="3">
         <v>1</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J14" s="12">
         <f t="shared" si="2"/>
         <v>189076</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K14" s="13">
         <f t="shared" si="0"/>
         <v>35924.44</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L14" s="13">
         <f t="shared" si="5"/>
         <v>225000.44</v>
       </c>
-      <c r="M10" s="22"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="22"/>
-      <c r="C11" s="5" t="s">
+      <c r="M14" s="31"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="31"/>
+      <c r="C15" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F15" s="5">
         <v>4</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G15" s="6">
         <v>109240</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H15" s="14">
         <f t="shared" si="1"/>
         <v>436960</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I15" s="5">
         <v>4</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J15" s="6">
         <f t="shared" si="2"/>
         <v>1747840</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K15" s="6">
         <f t="shared" si="0"/>
         <v>332089.59999999998</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L15" s="6">
         <f t="shared" si="5"/>
         <v>2079929.6</v>
       </c>
-      <c r="M11" s="22"/>
-    </row>
-    <row r="12" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B12" s="22" t="s">
+      <c r="M15" s="31"/>
+    </row>
+    <row r="16" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B16" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C16" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F16" s="3">
         <v>4</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G16" s="12">
         <v>1428600</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H16" s="12">
         <f t="shared" si="1"/>
         <v>5714400</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I16" s="3">
         <v>1</v>
       </c>
-      <c r="J12" s="13">
-        <f t="shared" ref="J12" si="6">H12*I12</f>
+      <c r="J16" s="13">
+        <f t="shared" ref="J16" si="6">H16*I16</f>
         <v>5714400</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K16" s="13">
         <f t="shared" si="0"/>
         <v>1085736</v>
       </c>
-      <c r="L12" s="15">
+      <c r="L16" s="15">
         <f t="shared" si="5"/>
         <v>6800136</v>
       </c>
-      <c r="M12" s="21">
-        <f>SUM(L12:L14)</f>
+      <c r="M16" s="28">
+        <f>SUM(L16:L18)</f>
         <v>9108736</v>
       </c>
     </row>
-    <row r="13" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B13" s="22"/>
-      <c r="C13" s="11" t="s">
+    <row r="17" spans="2:13" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B17" s="31"/>
+      <c r="C17" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F17" s="5">
         <v>4</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G17" s="6">
         <v>400000</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H17" s="6">
         <f t="shared" si="1"/>
         <v>1600000</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I17" s="5">
         <v>1</v>
       </c>
-      <c r="J13" s="6">
-        <f t="shared" ref="J13" si="7">H13*I13</f>
+      <c r="J17" s="6">
+        <f t="shared" ref="J17" si="7">H17*I17</f>
         <v>1600000</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K17" s="6">
         <f t="shared" si="0"/>
         <v>304000</v>
       </c>
-      <c r="L13" s="16">
+      <c r="L17" s="16">
         <f t="shared" si="5"/>
         <v>1904000</v>
       </c>
-      <c r="M13" s="22"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="22"/>
-      <c r="C14" s="3" t="s">
+      <c r="M17" s="31"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="31"/>
+      <c r="C18" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F18" s="3">
         <v>4</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G18" s="12">
         <v>85000</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H18" s="13">
         <f t="shared" si="1"/>
         <v>340000</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I18" s="3">
         <v>1</v>
       </c>
-      <c r="J14" s="13">
-        <f t="shared" ref="J14" si="8">H14*I14</f>
+      <c r="J18" s="13">
+        <f t="shared" ref="J18" si="8">H18*I18</f>
         <v>340000</v>
       </c>
-      <c r="K14" s="13">
+      <c r="K18" s="13">
         <f t="shared" si="0"/>
         <v>64600</v>
       </c>
-      <c r="L14" s="15">
+      <c r="L18" s="15">
         <f t="shared" si="5"/>
         <v>404600</v>
       </c>
-      <c r="M14" s="22"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="K15" s="25" t="s">
+      <c r="M18" s="31"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="K19" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="L15" s="25"/>
-      <c r="M15" s="27">
-        <f>SUM(M4:M14)</f>
+      <c r="L19" s="23"/>
+      <c r="M19" s="25">
+        <f>SUM(M8:M18)</f>
         <v>39883226.039999999</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="28"/>
-    </row>
-    <row r="17" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="K17" s="25" t="s">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="26"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="K21" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="L17" s="29">
+      <c r="L21" s="27">
         <v>0.05</v>
       </c>
-      <c r="M17" s="21">
-        <f>M15*L17</f>
+      <c r="M21" s="28">
+        <f>M19*L21</f>
         <v>1994161.3020000001</v>
       </c>
     </row>
-    <row r="18" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="K18" s="25"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="21"/>
-    </row>
-    <row r="19" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="K19" s="30" t="s">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K22" s="23"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="28"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K23" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="L19" s="30"/>
-      <c r="M19" s="31">
-        <f>M15+M17</f>
+      <c r="L23" s="29"/>
+      <c r="M23" s="30">
+        <f>M19+M21</f>
         <v>41877387.342</v>
       </c>
     </row>
-    <row r="20" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="31"/>
-    </row>
-    <row r="25" spans="4:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D25" s="23" t="s">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="30"/>
+    </row>
+    <row r="29" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="24"/>
-      <c r="G25" s="2" t="s">
+      <c r="E29" s="22"/>
+      <c r="G29" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H25" s="2"/>
-      <c r="I25" s="9">
+      <c r="H29" s="2"/>
+      <c r="I29" s="9">
         <v>0.19</v>
       </c>
-      <c r="J25" s="8"/>
-    </row>
-    <row r="26" spans="4:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="D26" s="2" t="s">
+      <c r="J29" s="8"/>
+    </row>
+    <row r="30" spans="2:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="D30" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E30" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="4:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="D27" s="2" t="s">
+    <row r="31" spans="2:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="D31" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E31" s="3">
         <v>6</v>
       </c>
-      <c r="G27" s="25" t="s">
+      <c r="G31" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-    </row>
-    <row r="28" spans="4:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="D28" s="2" t="s">
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+    </row>
+    <row r="32" spans="2:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="D32" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="3">
-        <f>E26*E27</f>
+      <c r="E32" s="3">
+        <f>E30*E31</f>
         <v>90</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H32" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="G29" s="7">
+    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="G33" s="7">
         <v>1</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H33" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="I33" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="4:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="D30" s="23" t="s">
+    <row r="34" spans="4:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="D34" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E30" s="24"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="4:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="D31" s="2" t="s">
+      <c r="E34" s="22"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+    </row>
+    <row r="35" spans="4:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="D35" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E35" s="3">
         <v>14</v>
       </c>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-    </row>
-    <row r="32" spans="4:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D32" s="2" t="s">
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="4:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D36" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E36" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="4:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="D33" s="2" t="s">
+    <row r="37" spans="4:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="D37" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="3">
-        <f>E31*E32</f>
+      <c r="E37" s="3">
+        <f>E35*E36</f>
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="4:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="D35" s="23" t="s">
+    <row r="39" spans="4:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="D39" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E35" s="24"/>
-    </row>
-    <row r="36" spans="4:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="D36" s="2" t="s">
+      <c r="E39" s="22"/>
+    </row>
+    <row r="40" spans="4:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="D40" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E40" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="4:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D37" s="2" t="s">
+    <row r="41" spans="4:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D41" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E41" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="4:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="D38" s="2" t="s">
+    <row r="42" spans="4:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="D42" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E38" s="3">
-        <f>E36*E37</f>
+      <c r="E42" s="3">
+        <f>E40*E41</f>
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="4:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="D40" s="23" t="s">
+    <row r="44" spans="4:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="D44" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E40" s="24"/>
-    </row>
-    <row r="41" spans="4:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="D41" s="2" t="s">
+      <c r="E44" s="22"/>
+    </row>
+    <row r="45" spans="4:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="D45" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E45" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="4:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="D42" s="2" t="s">
+    <row r="46" spans="4:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="D46" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E46" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="4:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="D43" s="2" t="s">
+    <row r="47" spans="4:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="D47" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E43" s="3">
-        <f>E41*E42</f>
+      <c r="E47" s="3">
+        <f>E45*E46</f>
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="4:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="D45" s="23" t="s">
+    <row r="49" spans="4:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="D49" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="E45" s="24"/>
-    </row>
-    <row r="46" spans="4:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="D46" s="2" t="s">
+      <c r="E49" s="22"/>
+    </row>
+    <row r="50" spans="4:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="D50" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E50" s="3">
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="4:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="D47" s="2" t="s">
+    <row r="51" spans="4:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="D51" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E51" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="4:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="D48" s="2" t="s">
+    <row r="52" spans="4:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="D52" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E48" s="3">
-        <f>E46*E47</f>
+      <c r="E52" s="3">
+        <f>E50*E51</f>
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="K15:L16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="M17:M18"/>
+  <mergeCells count="21">
+    <mergeCell ref="B1:M4"/>
+    <mergeCell ref="B5:M6"/>
+    <mergeCell ref="M8:M12"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="M13:M15"/>
+    <mergeCell ref="M16:M18"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="D44:E44"/>
     <mergeCell ref="K19:L20"/>
     <mergeCell ref="M19:M20"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="M4:M8"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="M9:M11"/>
-    <mergeCell ref="M12:M14"/>
-    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="K23:L24"/>
+    <mergeCell ref="M23:M24"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D29:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="L5 L7" formula="1"/>
+    <ignoredError sqref="L9 L11" formula="1"/>
   </ignoredErrors>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>